<commit_message>
initial and fix errors
</commit_message>
<xml_diff>
--- a/backend/src/main/resources/wind.xlsx
+++ b/backend/src/main/resources/wind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_repos\wind\backend\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project_repos\modeling\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -68,7 +68,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,10 +349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B100"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +463,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B14">
         <v>2.82</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B15">
         <v>2.16</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="B16">
         <v>3.17</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="B17">
         <v>2.09</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B18">
         <v>1.59</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="B19">
         <v>2.71</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="B20">
         <v>4.97</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="B21">
         <v>3.22</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="B22">
         <v>1.5</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="B23">
         <v>0.8</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="B24">
         <v>0.87</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="B25">
         <v>2.1800000000000002</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="B26">
         <v>1.86</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>125</v>
+        <v>205</v>
       </c>
       <c r="B27">
         <v>0.81</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="B28">
         <v>4.1500000000000004</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>135</v>
+        <v>215</v>
       </c>
       <c r="B29">
         <v>5.29</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="B30">
         <v>6.96</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>145</v>
+        <v>225</v>
       </c>
       <c r="B31">
         <v>5.56</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="B32">
         <v>5.65</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="B33">
         <v>4.47</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="B34">
         <v>1.38</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>165</v>
+        <v>245</v>
       </c>
       <c r="B35">
         <v>1.25</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="B36">
         <v>0.74</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>175</v>
+        <v>255</v>
       </c>
       <c r="B37">
         <v>1.66</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="B38">
         <v>3.09</v>
@@ -663,7 +663,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>185</v>
+        <v>305</v>
       </c>
       <c r="B39">
         <v>2.5099999999999998</v>
@@ -671,7 +671,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="B40">
         <v>2.04</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>195</v>
+        <v>315</v>
       </c>
       <c r="B41">
         <v>4.3</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>200</v>
+        <v>320</v>
       </c>
       <c r="B42">
         <v>8.1300000000000008</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>205</v>
+        <v>325</v>
       </c>
       <c r="B43">
         <v>8.86</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>210</v>
+        <v>330</v>
       </c>
       <c r="B44">
         <v>2.39</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>215</v>
+        <v>335</v>
       </c>
       <c r="B45">
         <v>0.34</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>220</v>
+        <v>340</v>
       </c>
       <c r="B46">
         <v>1.05</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>225</v>
+        <v>345</v>
       </c>
       <c r="B47">
         <v>0.23</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>230</v>
+        <v>350</v>
       </c>
       <c r="B48">
         <v>0.96</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>235</v>
+        <v>355</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>240</v>
+        <v>400</v>
       </c>
       <c r="B50">
         <v>3.94</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>245</v>
+        <v>405</v>
       </c>
       <c r="B51">
         <v>5.92</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>250</v>
+        <v>410</v>
       </c>
       <c r="B52">
         <v>1.93</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>255</v>
+        <v>415</v>
       </c>
       <c r="B53">
         <v>1.91</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>260</v>
+        <v>420</v>
       </c>
       <c r="B54">
         <v>2.41</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>265</v>
+        <v>425</v>
       </c>
       <c r="B55">
         <v>6.11</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>270</v>
+        <v>430</v>
       </c>
       <c r="B56">
         <v>5.49</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>275</v>
+        <v>435</v>
       </c>
       <c r="B57">
         <v>7.25</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>280</v>
+        <v>440</v>
       </c>
       <c r="B58">
         <v>10.28</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>285</v>
+        <v>445</v>
       </c>
       <c r="B59">
         <v>9.31</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>290</v>
+        <v>450</v>
       </c>
       <c r="B60">
         <v>8.07</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>295</v>
+        <v>455</v>
       </c>
       <c r="B61">
         <v>9.75</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>300</v>
+        <v>500</v>
       </c>
       <c r="B62">
         <v>7.82</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>305</v>
+        <v>505</v>
       </c>
       <c r="B63">
         <v>5.6</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>310</v>
+        <v>510</v>
       </c>
       <c r="B64">
         <v>2.33</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>315</v>
+        <v>515</v>
       </c>
       <c r="B65">
         <v>1.38</v>
@@ -879,7 +879,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>320</v>
+        <v>520</v>
       </c>
       <c r="B66">
         <v>0.51</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>325</v>
+        <v>525</v>
       </c>
       <c r="B67">
         <v>2.56</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>330</v>
+        <v>530</v>
       </c>
       <c r="B68">
         <v>5.71</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>335</v>
+        <v>535</v>
       </c>
       <c r="B69">
         <v>4.29</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>340</v>
+        <v>540</v>
       </c>
       <c r="B70">
         <v>4.1500000000000004</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>345</v>
+        <v>545</v>
       </c>
       <c r="B71">
         <v>2.92</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>350</v>
+        <v>550</v>
       </c>
       <c r="B72">
         <v>1.61</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>355</v>
+        <v>555</v>
       </c>
       <c r="B73">
         <v>4.09</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>360</v>
+        <v>600</v>
       </c>
       <c r="B74">
         <v>4.6900000000000004</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>365</v>
+        <v>605</v>
       </c>
       <c r="B75">
         <v>3.29</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>370</v>
+        <v>610</v>
       </c>
       <c r="B76">
         <v>2.5099999999999998</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>375</v>
+        <v>615</v>
       </c>
       <c r="B77">
         <v>4.04</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>380</v>
+        <v>620</v>
       </c>
       <c r="B78">
         <v>1.99</v>
@@ -983,7 +983,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>385</v>
+        <v>625</v>
       </c>
       <c r="B79">
         <v>4.43</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>390</v>
+        <v>630</v>
       </c>
       <c r="B80">
         <v>3.36</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>395</v>
+        <v>635</v>
       </c>
       <c r="B81">
         <v>4.8</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>400</v>
+        <v>640</v>
       </c>
       <c r="B82">
         <v>3.76</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>405</v>
+        <v>645</v>
       </c>
       <c r="B83">
         <v>5.37</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>410</v>
+        <v>650</v>
       </c>
       <c r="B84">
         <v>4.0999999999999996</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>415</v>
+        <v>655</v>
       </c>
       <c r="B85">
         <v>0.7</v>
@@ -1039,7 +1039,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>420</v>
+        <v>700</v>
       </c>
       <c r="B86">
         <v>1.54</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>425</v>
+        <v>705</v>
       </c>
       <c r="B87">
         <v>1.28</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>430</v>
+        <v>710</v>
       </c>
       <c r="B88">
         <v>0.47</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>435</v>
+        <v>715</v>
       </c>
       <c r="B89">
         <v>0.56000000000000005</v>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>440</v>
+        <v>720</v>
       </c>
       <c r="B90">
         <v>0.53</v>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>445</v>
+        <v>725</v>
       </c>
       <c r="B91">
         <v>1.0900000000000001</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>450</v>
+        <v>730</v>
       </c>
       <c r="B92">
         <v>0.75</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>455</v>
+        <v>735</v>
       </c>
       <c r="B93">
         <v>0.46</v>
@@ -1103,7 +1103,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>460</v>
+        <v>740</v>
       </c>
       <c r="B94">
         <v>0.53</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>465</v>
+        <v>745</v>
       </c>
       <c r="B95">
         <v>1.35</v>
@@ -1119,7 +1119,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>470</v>
+        <v>750</v>
       </c>
       <c r="B96">
         <v>1.01</v>
@@ -1127,7 +1127,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>475</v>
+        <v>755</v>
       </c>
       <c r="B97">
         <v>1.58</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>480</v>
+        <v>800</v>
       </c>
       <c r="B98">
         <v>3.13</v>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>485</v>
+        <v>805</v>
       </c>
       <c r="B99">
         <v>6.31</v>
@@ -1151,11 +1151,14 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>490</v>
+        <v>810</v>
       </c>
       <c r="B100">
         <v>0.71</v>
       </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>